<commit_message>
fix Rule hoạt động.xlsx
</commit_message>
<xml_diff>
--- a/Documents/Other/Rule hoạt động.xlsx
+++ b/Documents/Other/Rule hoạt động.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Capstone Project Home\DATN_OutSourcingHRM\trunk\Documents\Other\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\FU\Summer2015\DATN\DATN_OutSourcingHRM\trunk\Documents\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="19095" windowHeight="8445"/>
+    <workbookView xWindow="1065" yWindow="60" windowWidth="19095" windowHeight="8445"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
   <si>
     <t xml:space="preserve">CAPSTONE PROJECT </t>
   </si>
@@ -210,6 +210,9 @@
   </si>
   <si>
     <t>ok</t>
+  </si>
+  <si>
+    <t>KienNT</t>
   </si>
 </sst>
 </file>
@@ -595,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K53"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="H54" sqref="H54"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,6 +883,14 @@
         <v>61</v>
       </c>
       <c r="I53" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H54" t="s">
+        <v>63</v>
+      </c>
+      <c r="I54" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>